<commit_message>
fixed plotting and increase iterations
</commit_message>
<xml_diff>
--- a/Output/AllModels_experimental_noAR.xlsx
+++ b/Output/AllModels_experimental_noAR.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="434">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -101,465 +101,468 @@
     <t xml:space="preserve">0.868</t>
   </si>
   <si>
+    <t xml:space="preserve">0.012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very Strong Evidence for Null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conditional Within-Person Effects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily persuasion experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.97,  1.08]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.828</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  1.00,   1.06]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.966</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strong Evidence for Null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.04, 0.05]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.553</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.85*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.71,  0.99]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.253</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moderate Evidence for Null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.69,   1.01]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.199</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily persuasion utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.98,  1.08]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.899</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.99,   1.05]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.888</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.02, 0.07]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.829</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.84,  1.24]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.607</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.85,   1.54]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.077</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily pressure experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.89*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.80,  0.99]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.984</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.484</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weak Evidence for Null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.88,   1.01]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.960</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.14, 0.07]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.767</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.84*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.18,  2.68]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.366</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moderate Evidence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.04*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.03,   4.57]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.979</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.451</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weak Evidence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily pressure utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.86,  1.03]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.915</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.92,   1.05]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.714</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.14, 0.08]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.661</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.011</t>
   </si>
   <si>
-    <t xml:space="preserve">Very Strong Evidence for Null</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conditional Within-Person Effects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily persuasion experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.97,  1.08]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.828</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  1.00,   1.06]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.966</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.035</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Strong Evidence for Null</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.04, 0.05]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.553</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.85*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.71,  0.99]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.980</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.249</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moderate Evidence for Null</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.69,   1.01]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.197</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily persuasion utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.98,  1.08]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.899</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.036</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.99,   1.05]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.888</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.02, 0.07]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.829</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.84,  1.24]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.607</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.040</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.85,   1.54]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.789</t>
+    <t xml:space="preserve">1.22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.71,  2.06]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.149</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.58,   4.04]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.799</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.251</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily pushing experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.96,  1.10]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.775</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.98,   1.08]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.04, 0.09]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.768</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.97,  1.43]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.946</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.28*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.01,   1.64]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily pushing utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.93,  1.05]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.618</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.97,   1.06]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.771</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.08*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.01, 0.14]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.71,  1.17]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.770</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.064</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.60,   1.31]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.735</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.096</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.89,  1.13]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.551</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.91,   1.04]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.785</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.26*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.15, 0.37]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50.164</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very Strong Evidence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.75,  2.89]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.871</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.256</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.77,   3.51]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.364</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily weartime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.00*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  1.00,   1.00]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conditional Between-Person Effects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean persuasion experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.74,  1.38]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.533</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.82,   1.46]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.748</t>
   </si>
   <si>
     <t xml:space="preserve">0.075</t>
   </si>
   <si>
-    <t xml:space="preserve">Daily pressure experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.89*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.80,  0.99]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.984</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.483</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weak Evidence for Null</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.94</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.88,   1.01]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.960</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.074</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.14, 0.07]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.767</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.84*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1.18,  2.68]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.994</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.405</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moderate Evidence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.04*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1.03,   4.57]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.979</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.426</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weak Evidence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily pressure utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.86,  1.03]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.915</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.98</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.92,   1.05]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.714</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.14, 0.08]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.661</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.71,  2.06]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.808</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.148</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.58,   4.04]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.799</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.247</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily pushing experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.96,  1.10]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.775</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.033</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.98,   1.08]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.900</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.04, 0.09]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.768</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.97,  1.43]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.946</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.149</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.28*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1.01,   1.64]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.409</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily pushing utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.93,  1.05]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.618</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.97,   1.06]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.771</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.08*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.01, 0.14]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.078</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.91</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.71,  1.17]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.770</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.064</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.89</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.60,   1.31]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.735</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.094</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.89,  1.13]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.551</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.041</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.97</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.91,   1.04]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.785</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.26*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.15, 0.37]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">52.056</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very Strong Evidence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.75,  2.89]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.871</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.257</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.77,   3.51]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.358</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily weartime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.00*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  1.00,   1.00]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conditional Between-Person Effects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean persuasion experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.74,  1.38]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.533</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.82,   1.46]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.748</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.33</t>
   </si>
   <si>
@@ -569,7 +572,7 @@
     <t xml:space="preserve">0.889</t>
   </si>
   <si>
-    <t xml:space="preserve">0.120</t>
+    <t xml:space="preserve">0.118</t>
   </si>
   <si>
     <t xml:space="preserve">1.12</t>
@@ -581,7 +584,7 @@
     <t xml:space="preserve">0.586</t>
   </si>
   <si>
-    <t xml:space="preserve">0.208</t>
+    <t xml:space="preserve">0.204</t>
   </si>
   <si>
     <t xml:space="preserve">1.99</t>
@@ -593,7 +596,7 @@
     <t xml:space="preserve">0.870</t>
   </si>
   <si>
-    <t xml:space="preserve">0.471</t>
+    <t xml:space="preserve">0.454</t>
   </si>
   <si>
     <t xml:space="preserve">Mean persuasion utilized (partner's view)</t>
@@ -605,7 +608,7 @@
     <t xml:space="preserve">0.543</t>
   </si>
   <si>
-    <t xml:space="preserve">0.105</t>
+    <t xml:space="preserve">0.106</t>
   </si>
   <si>
     <t xml:space="preserve">[  0.73,   1.30]</t>
@@ -614,7 +617,7 @@
     <t xml:space="preserve">0.559</t>
   </si>
   <si>
-    <t xml:space="preserve">0.061</t>
+    <t xml:space="preserve">0.060</t>
   </si>
   <si>
     <t xml:space="preserve">0.22</t>
@@ -626,7 +629,7 @@
     <t xml:space="preserve">0.790</t>
   </si>
   <si>
-    <t xml:space="preserve">0.077</t>
+    <t xml:space="preserve">0.076</t>
   </si>
   <si>
     <t xml:space="preserve">1.38</t>
@@ -638,7 +641,7 @@
     <t xml:space="preserve">0.711</t>
   </si>
   <si>
-    <t xml:space="preserve">0.255</t>
+    <t xml:space="preserve">0.262</t>
   </si>
   <si>
     <t xml:space="preserve">1.90</t>
@@ -647,7 +650,7 @@
     <t xml:space="preserve">[0.52,   7.15]</t>
   </si>
   <si>
-    <t xml:space="preserve">0.401</t>
+    <t xml:space="preserve">0.417</t>
   </si>
   <si>
     <t xml:space="preserve">Mean pressure experienced</t>
@@ -662,7 +665,7 @@
     <t xml:space="preserve">0.772</t>
   </si>
   <si>
-    <t xml:space="preserve">0.153</t>
+    <t xml:space="preserve">0.158</t>
   </si>
   <si>
     <t xml:space="preserve">[  0.73,   1.31]</t>
@@ -671,7 +674,7 @@
     <t xml:space="preserve">0.560</t>
   </si>
   <si>
-    <t xml:space="preserve">0.060</t>
+    <t xml:space="preserve">0.062</t>
   </si>
   <si>
     <t xml:space="preserve">-0.31</t>
@@ -683,7 +686,7 @@
     <t xml:space="preserve">0.874</t>
   </si>
   <si>
-    <t xml:space="preserve">0.102</t>
+    <t xml:space="preserve">0.101</t>
   </si>
   <si>
     <t xml:space="preserve">3.51*</t>
@@ -695,7 +698,7 @@
     <t xml:space="preserve">0.990</t>
   </si>
   <si>
-    <t xml:space="preserve">3.276</t>
+    <t xml:space="preserve">3.142</t>
   </si>
   <si>
     <t xml:space="preserve">17.91*</t>
@@ -707,7 +710,7 @@
     <t xml:space="preserve">0.997</t>
   </si>
   <si>
-    <t xml:space="preserve">19.951</t>
+    <t xml:space="preserve">20.152</t>
   </si>
   <si>
     <t xml:space="preserve">Strong Evidence</t>
@@ -722,15 +725,15 @@
     <t xml:space="preserve">0.744</t>
   </si>
   <si>
+    <t xml:space="preserve">0.155</t>
+  </si>
+  <si>
     <t xml:space="preserve">[  0.73,   1.28]</t>
   </si>
   <si>
     <t xml:space="preserve">0.594</t>
   </si>
   <si>
-    <t xml:space="preserve">0.058</t>
-  </si>
-  <si>
     <t xml:space="preserve">-0.30</t>
   </si>
   <si>
@@ -746,7 +749,7 @@
     <t xml:space="preserve">0.612</t>
   </si>
   <si>
-    <t xml:space="preserve">0.237</t>
+    <t xml:space="preserve">0.239</t>
   </si>
   <si>
     <t xml:space="preserve">2.27</t>
@@ -758,7 +761,7 @@
     <t xml:space="preserve">0.769</t>
   </si>
   <si>
-    <t xml:space="preserve">0.587</t>
+    <t xml:space="preserve">0.597</t>
   </si>
   <si>
     <t xml:space="preserve">Mean pushing experienced</t>
@@ -773,18 +776,21 @@
     <t xml:space="preserve">0.891</t>
   </si>
   <si>
-    <t xml:space="preserve">0.312</t>
+    <t xml:space="preserve">0.322</t>
   </si>
   <si>
     <t xml:space="preserve">[  0.65,   1.45]</t>
   </si>
   <si>
-    <t xml:space="preserve">0.082</t>
+    <t xml:space="preserve">0.080</t>
   </si>
   <si>
     <t xml:space="preserve">[-0.54, 0.99]</t>
   </si>
   <si>
+    <t xml:space="preserve">0.091</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.23</t>
   </si>
   <si>
@@ -794,7 +800,7 @@
     <t xml:space="preserve">0.605</t>
   </si>
   <si>
-    <t xml:space="preserve">0.300</t>
+    <t xml:space="preserve">0.308</t>
   </si>
   <si>
     <t xml:space="preserve">0.83</t>
@@ -806,6 +812,9 @@
     <t xml:space="preserve">0.580</t>
   </si>
   <si>
+    <t xml:space="preserve">0.405</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mean pushing utilized (partner's view)</t>
   </si>
   <si>
@@ -818,9 +827,6 @@
     <t xml:space="preserve">0.925</t>
   </si>
   <si>
-    <t xml:space="preserve">0.441</t>
-  </si>
-  <si>
     <t xml:space="preserve">1.25</t>
   </si>
   <si>
@@ -830,7 +836,7 @@
     <t xml:space="preserve">0.859</t>
   </si>
   <si>
-    <t xml:space="preserve">0.146</t>
+    <t xml:space="preserve">0.152</t>
   </si>
   <si>
     <t xml:space="preserve">0.35</t>
@@ -842,7 +848,7 @@
     <t xml:space="preserve">0.825</t>
   </si>
   <si>
-    <t xml:space="preserve">0.118</t>
+    <t xml:space="preserve">0.121</t>
   </si>
   <si>
     <t xml:space="preserve">0.11*</t>
@@ -854,13 +860,13 @@
     <t xml:space="preserve">0.992</t>
   </si>
   <si>
-    <t xml:space="preserve">7.844</t>
+    <t xml:space="preserve">7.898</t>
   </si>
   <si>
     <t xml:space="preserve">[0.01,   0.66]</t>
   </si>
   <si>
-    <t xml:space="preserve">7.231</t>
+    <t xml:space="preserve">7.042</t>
   </si>
   <si>
     <t xml:space="preserve">Mean weartime</t>
@@ -905,9 +911,6 @@
     <t xml:space="preserve">0.898</t>
   </si>
   <si>
-    <t xml:space="preserve">0.155</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hu Daily pressure utilized (partner's view)</t>
   </si>
   <si>
@@ -920,97 +923,103 @@
     <t xml:space="preserve">0.988</t>
   </si>
   <si>
+    <t xml:space="preserve">0.890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Daily pushing experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.58*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.40,  0.78]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.195</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Daily pushing utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.54*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.41,  0.69]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.85,  1.42]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.750</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Daily weartime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hurdle Between-Person Effects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Mean persuasion experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.36,  1.87]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.680</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.183</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Mean persuasion utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.36,  1.89]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.671</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Mean pressure experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.31*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 1.36,  8.35]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Mean pressure utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.74,  4.48]</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.905</t>
   </si>
   <si>
-    <t xml:space="preserve">Hu Daily pushing experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.58*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.40,  0.78]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24.738</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Daily pushing utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.54*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.41,  0.69]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.85,  1.42]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.750</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.066</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Daily weartime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hurdle Between-Person Effects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Mean persuasion experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.36,  1.87]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.680</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.182</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Mean persuasion utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.36,  1.89]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.671</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Mean pressure experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.31*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 1.36,  8.35]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.995</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.938</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Mean pressure utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.79</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.74,  4.48]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.435</t>
+    <t xml:space="preserve">0.428</t>
   </si>
   <si>
     <t xml:space="preserve">Hu Mean pushing experienced</t>
@@ -1022,7 +1031,7 @@
     <t xml:space="preserve">0.962</t>
   </si>
   <si>
-    <t xml:space="preserve">1.154</t>
+    <t xml:space="preserve">1.141</t>
   </si>
   <si>
     <t xml:space="preserve">Hu Mean pushing utilized (partner's view)</t>
@@ -1037,7 +1046,7 @@
     <t xml:space="preserve">0.964</t>
   </si>
   <si>
-    <t xml:space="preserve">1.276</t>
+    <t xml:space="preserve">1.261</t>
   </si>
   <si>
     <t xml:space="preserve">Hu Mean weartime</t>
@@ -2321,7 +2330,7 @@
         <v>98</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>40</v>
@@ -2776,52 +2785,52 @@
         <v>181</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>81</v>
+        <v>182</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>40</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>49</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="U15" s="1" t="s">
         <v>49</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="Z15" s="1" t="s">
         <v>77</v>
@@ -2829,19 +2838,19 @@
     </row>
     <row r="16">
       <c r="A16" s="9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>99</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>49</v>
@@ -2850,58 +2859,58 @@
         <v>99</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>40</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="P16" s="1" t="s">
         <v>40</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="U16" s="1" t="s">
         <v>49</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="X16" s="1" t="s">
         <v>63</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="Z16" s="1" t="s">
         <v>77</v>
@@ -2909,19 +2918,19 @@
     </row>
     <row r="17">
       <c r="A17" s="9" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>49</v>
@@ -2930,78 +2939,78 @@
         <v>99</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>40</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="P17" s="1" t="s">
         <v>49</v>
       </c>
       <c r="Q17" s="5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="U17" s="1" t="s">
         <v>90</v>
       </c>
       <c r="V17" s="5" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="X17" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="Z17" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="9" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>146</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>216</v>
+        <v>237</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>49</v>
@@ -3010,28 +3019,28 @@
         <v>155</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>238</v>
+        <v>201</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>40</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>165</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="P18" s="1" t="s">
         <v>40</v>
@@ -3040,28 +3049,28 @@
         <v>125</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="U18" s="1" t="s">
         <v>49</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="X18" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="Z18" s="1" t="s">
         <v>77</v>
@@ -3069,19 +3078,19 @@
     </row>
     <row r="19">
       <c r="A19" s="9" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>77</v>
@@ -3090,58 +3099,58 @@
         <v>155</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>40</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>101</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>149</v>
+        <v>258</v>
       </c>
       <c r="P19" s="1" t="s">
         <v>40</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="X19" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="Y19" s="1" t="s">
-        <v>131</v>
+        <v>266</v>
       </c>
       <c r="Z19" s="1" t="s">
         <v>77</v>
@@ -3149,64 +3158,64 @@
     </row>
     <row r="20">
       <c r="A20" s="9" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>268</v>
+        <v>194</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>77</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>49</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="P20" s="1" t="s">
         <v>49</v>
       </c>
       <c r="Q20" s="5" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="U20" s="1" t="s">
         <v>90</v>
@@ -3215,13 +3224,13 @@
         <v>139</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="X20" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="Z20" s="1" t="s">
         <v>90</v>
@@ -3229,7 +3238,7 @@
     </row>
     <row r="21">
       <c r="A21" s="9" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -3237,16 +3246,16 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>172</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>30</v>
@@ -3269,93 +3278,93 @@
     </row>
     <row r="22">
       <c r="A22" s="8" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="X22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="Z22" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="9" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>16</v>
@@ -3389,13 +3398,13 @@
     </row>
     <row r="24">
       <c r="A24" s="9" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>16</v>
@@ -3429,19 +3438,19 @@
     </row>
     <row r="25">
       <c r="A25" s="9" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>297</v>
+        <v>274</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>49</v>
@@ -3469,19 +3478,19 @@
     </row>
     <row r="26">
       <c r="A26" s="9" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>77</v>
@@ -3509,22 +3518,22 @@
     </row>
     <row r="27">
       <c r="A27" s="9" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -3549,13 +3558,13 @@
     </row>
     <row r="28">
       <c r="A28" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>16</v>
@@ -3589,19 +3598,19 @@
     </row>
     <row r="29">
       <c r="A29" s="9" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>40</v>
@@ -3629,7 +3638,7 @@
     </row>
     <row r="30">
       <c r="A30" s="9" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -3659,99 +3668,99 @@
     </row>
     <row r="31">
       <c r="A31" s="8" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="T31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="U31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="V31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="W31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="X31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="Y31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="Z31" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="9" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>49</v>
@@ -3779,19 +3788,19 @@
     </row>
     <row r="33">
       <c r="A33" s="9" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>49</v>
@@ -3819,19 +3828,19 @@
     </row>
     <row r="34">
       <c r="A34" s="9" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>90</v>
@@ -3859,19 +3868,19 @@
     </row>
     <row r="35">
       <c r="A35" s="9" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>302</v>
+        <v>334</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>77</v>
@@ -3899,19 +3908,19 @@
     </row>
     <row r="36">
       <c r="A36" s="9" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>95</v>
@@ -3939,19 +3948,19 @@
     </row>
     <row r="37">
       <c r="A37" s="9" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>95</v>
@@ -3979,7 +3988,7 @@
     </row>
     <row r="38">
       <c r="A38" s="9" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -4009,129 +4018,129 @@
     </row>
     <row r="39">
       <c r="A39" s="8" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="S39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="T39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="U39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="V39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="W39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="X39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="Y39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="Z39" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="9" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
       <c r="Q40" s="1" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="R40" s="1" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
       <c r="U40" s="1"/>
       <c r="V40" s="1" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="W40" s="1" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="X40" s="1"/>
       <c r="Y40" s="1"/>
@@ -4139,13 +4148,13 @@
     </row>
     <row r="41">
       <c r="A41" s="9" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -4173,49 +4182,49 @@
     </row>
     <row r="42">
       <c r="A42" s="9" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
       <c r="Q42" s="1" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="R42" s="1" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
       <c r="V42" s="1" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="W42" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="X42" s="1"/>
       <c r="Y42" s="1"/>
@@ -4223,49 +4232,49 @@
     </row>
     <row r="43">
       <c r="A43" s="9" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
       <c r="Q43" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="R43" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
       <c r="U43" s="1"/>
       <c r="V43" s="1" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="W43" s="1" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="X43" s="1"/>
       <c r="Y43" s="1"/>
@@ -4273,49 +4282,49 @@
     </row>
     <row r="44">
       <c r="A44" s="9" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
       <c r="Q44" s="1" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="R44" s="1" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
       <c r="U44" s="1"/>
       <c r="V44" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="W44" s="1" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="X44" s="1"/>
       <c r="Y44" s="1"/>
@@ -4323,40 +4332,40 @@
     </row>
     <row r="45">
       <c r="A45" s="9" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
       <c r="Q45" s="1" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="R45" s="1" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="S45" s="1"/>
       <c r="T45" s="1"/>
@@ -4365,7 +4374,7 @@
         <v>155</v>
       </c>
       <c r="W45" s="1" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="X45" s="1"/>
       <c r="Y45" s="1"/>
@@ -4373,49 +4382,49 @@
     </row>
     <row r="46">
       <c r="A46" s="9" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
       <c r="Q46" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="R46" s="1" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="S46" s="1"/>
       <c r="T46" s="1"/>
       <c r="U46" s="1"/>
       <c r="V46" s="1" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="W46" s="1" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="X46" s="1"/>
       <c r="Y46" s="1"/>
@@ -4423,49 +4432,49 @@
     </row>
     <row r="47">
       <c r="A47" s="9" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
       <c r="Q47" s="1" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="R47" s="1" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="S47" s="1"/>
       <c r="T47" s="1"/>
       <c r="U47" s="1"/>
       <c r="V47" s="1" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="W47" s="1" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="X47" s="1"/>
       <c r="Y47" s="1"/>
@@ -4473,13 +4482,13 @@
     </row>
     <row r="48">
       <c r="A48" s="9" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -4507,13 +4516,13 @@
     </row>
     <row r="49">
       <c r="A49" s="9" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -4541,13 +4550,13 @@
     </row>
     <row r="50">
       <c r="A50" s="9" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -4575,13 +4584,13 @@
     </row>
     <row r="51">
       <c r="A51" s="9" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -4609,13 +4618,13 @@
     </row>
     <row r="52">
       <c r="A52" s="9" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -4643,13 +4652,13 @@
     </row>
     <row r="53">
       <c r="A53" s="9" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -4677,87 +4686,87 @@
     </row>
     <row r="54">
       <c r="A54" s="8" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="R54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="S54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="T54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="U54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="V54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="W54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="X54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="Y54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="Z54" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="9" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -4787,7 +4796,7 @@
     </row>
     <row r="56">
       <c r="A56" s="9" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -4817,7 +4826,7 @@
     </row>
     <row r="57">
       <c r="A57" s="9" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -4847,7 +4856,7 @@
     </row>
     <row r="58">
       <c r="A58" s="9" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -4877,7 +4886,7 @@
     </row>
     <row r="59">
       <c r="A59" s="9" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -4907,7 +4916,7 @@
     </row>
     <row r="60">
       <c r="A60" s="9" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -4937,31 +4946,31 @@
     </row>
     <row r="61">
       <c r="A61" s="10" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
       <c r="G61" s="4" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
       <c r="L61" s="4" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="M61" s="4" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="N61" s="6"/>
       <c r="O61" s="6"/>

</xml_diff>